<commit_message>
Updated calibration metrics for 2023
</commit_message>
<xml_diff>
--- a/files/cali_summary_2022-07_29_new_modules.xlsx
+++ b/files/cali_summary_2022-07_29_new_modules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\chl_qc\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B7DD5C-2DEC-4094-A136-E8AEEAB9DEAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4912472-8A21-4DB4-B596-1775A8C82016}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14604" activeTab="1" xr2:uid="{58D8BF88-922C-47DB-AA1D-0750D9F9DE65}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -132,9 +132,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -145,6 +142,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D756CCA0-DA7E-4572-A3CD-26843A1D1768}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,34 +479,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -543,7 +543,7 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>720001154</v>
       </c>
       <c r="D3" s="5">
@@ -615,58 +615,102 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>720000982</v>
+      </c>
+      <c r="D6" s="5">
+        <v>74672.33</v>
+      </c>
+      <c r="E6" s="16">
+        <v>79305.710000000006</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.7218121259655259</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3.4881475781258918E-4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.99993977709377369</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>720001154</v>
+      </c>
+      <c r="D7" s="5">
+        <v>100649.63</v>
+      </c>
+      <c r="E7" s="5">
+        <v>103637.64</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.7204263886038496</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7562378481617607E-4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.9999924834744941</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="I9" s="12"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="I10" s="12"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="I13" s="12"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="I15" s="12"/>
+      <c r="I15" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -676,20 +720,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297A9660-58AB-44EA-B3B6-7AC55341B8F5}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
@@ -701,8 +745,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44652</v>
       </c>
@@ -716,7 +763,7 @@
         <v>249.73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44652</v>
       </c>
@@ -729,8 +776,11 @@
       <c r="D3">
         <v>4529.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1.7450341655930464</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44652</v>
       </c>
@@ -743,8 +793,11 @@
       <c r="D4">
         <v>22357.33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1.7468920357254893</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44652</v>
       </c>
@@ -757,8 +810,11 @@
       <c r="D5">
         <v>54820.74</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1.7337625986958736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44652</v>
       </c>
@@ -771,8 +827,11 @@
       <c r="D6">
         <v>109397.75999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1.7356565631026306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44652</v>
       </c>
@@ -785,8 +844,11 @@
       <c r="D7">
         <v>161512.79</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1.7488504882666245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44652</v>
       </c>
@@ -799,8 +861,11 @@
       <c r="D8">
         <v>318181.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1.7628562549019229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44652</v>
       </c>
@@ -813,8 +878,11 @@
       <c r="D9">
         <v>646359.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1.7658015869515062</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44652</v>
       </c>
@@ -828,7 +896,7 @@
         <v>308.58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44652</v>
       </c>
@@ -841,8 +909,11 @@
       <c r="D11">
         <v>5983.49</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1.7443764101239985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44652</v>
       </c>
@@ -855,8 +926,11 @@
       <c r="D12">
         <v>29351.13</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1.72553405758999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44652</v>
       </c>
@@ -869,8 +943,11 @@
       <c r="D13">
         <v>72458.97</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1.7373700621572985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44652</v>
       </c>
@@ -883,8 +960,11 @@
       <c r="D14">
         <v>147773.09</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>1.7502048825970795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44652</v>
       </c>
@@ -897,8 +977,11 @@
       <c r="D15">
         <v>217388.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>1.77554336161815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44652</v>
       </c>
@@ -911,8 +994,11 @@
       <c r="D16">
         <v>427942.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1.7591003409279151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44652</v>
       </c>
@@ -925,8 +1011,11 @@
       <c r="D17">
         <v>877474.93</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1.7778380659784827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44726</v>
       </c>
@@ -940,7 +1029,7 @@
         <v>259.99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44726</v>
       </c>
@@ -953,8 +1042,11 @@
       <c r="D19">
         <v>4718.6899999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1.7294452137418495</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44726</v>
       </c>
@@ -967,8 +1059,11 @@
       <c r="D20">
         <v>22287.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1.7321614066265887</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44726</v>
       </c>
@@ -981,8 +1076,11 @@
       <c r="D21">
         <v>54558.71</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>1.7267690816456656</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44726</v>
       </c>
@@ -995,8 +1093,11 @@
       <c r="D22">
         <v>106393.54</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>1.7277588804536006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44726</v>
       </c>
@@ -1009,8 +1110,11 @@
       <c r="D23">
         <v>162487.67999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1.7416364723602662</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44726</v>
       </c>
@@ -1023,8 +1127,11 @@
       <c r="D24">
         <v>326799.25</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>1.7595403307667432</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44726</v>
       </c>
@@ -1037,8 +1144,11 @@
       <c r="D25">
         <v>641608.06000000006</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>1.7664507643368839</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44726</v>
       </c>
@@ -1052,7 +1162,7 @@
         <v>299.58</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44726</v>
       </c>
@@ -1065,8 +1175,11 @@
       <c r="D27">
         <v>6321.57</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>1.6969040326193852</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44726</v>
       </c>
@@ -1079,8 +1192,11 @@
       <c r="D28">
         <v>29990.58</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>1.7181178071791645</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44726</v>
       </c>
@@ -1093,8 +1209,11 @@
       <c r="D29">
         <v>72982.58</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1.7283028828034064</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44726</v>
       </c>
@@ -1107,8 +1226,11 @@
       <c r="D30">
         <v>142588.71</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>1.7304599665872882</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44726</v>
       </c>
@@ -1121,8 +1243,11 @@
       <c r="D31">
         <v>219285.39</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>1.758870744662566</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44726</v>
       </c>
@@ -1135,8 +1260,11 @@
       <c r="D32">
         <v>444711.09</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>1.7625096074908684</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44726</v>
       </c>
@@ -1149,8 +1277,275 @@
       <c r="D33">
         <v>873760.87</v>
       </c>
+      <c r="E33">
+        <v>1.7773844974964832</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B34">
+        <v>720001154</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B35">
+        <v>720001154</v>
+      </c>
+      <c r="C35">
+        <v>2.0531538724763321</v>
+      </c>
+      <c r="D35">
+        <v>4566.5600000000004</v>
+      </c>
+      <c r="E35">
+        <v>1.7193470762813832</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B36">
+        <v>720001154</v>
+      </c>
+      <c r="C36">
+        <v>10.265769362381659</v>
+      </c>
+      <c r="D36">
+        <v>21504.61</v>
+      </c>
+      <c r="E36">
+        <v>1.7124794765356794</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B37">
+        <v>720001154</v>
+      </c>
+      <c r="C37">
+        <v>25.66442340595415</v>
+      </c>
+      <c r="D37">
+        <v>52627.38</v>
+      </c>
+      <c r="E37">
+        <v>1.7121035507254907</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B38">
+        <v>720001154</v>
+      </c>
+      <c r="C38">
+        <v>49.7547621763431</v>
+      </c>
+      <c r="D38">
+        <v>104570.07</v>
+      </c>
+      <c r="E38">
+        <v>1.7076299840552152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B39">
+        <v>720001154</v>
+      </c>
+      <c r="C39">
+        <v>74.632143264514653</v>
+      </c>
+      <c r="D39">
+        <v>155803.57</v>
+      </c>
+      <c r="E39">
+        <v>1.71324481724375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B40">
+        <v>720001154</v>
+      </c>
+      <c r="C40">
+        <v>149.26428652902931</v>
+      </c>
+      <c r="D40">
+        <v>313015.25</v>
+      </c>
+      <c r="E40">
+        <v>1.7339053107497115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B41">
+        <v>720001154</v>
+      </c>
+      <c r="C41">
+        <v>298.52857305805861</v>
+      </c>
+      <c r="D41">
+        <v>627502.18000000005</v>
+      </c>
+      <c r="E41">
+        <v>1.7442745046357175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B42">
+        <v>720000982</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B43">
+        <v>720000982</v>
+      </c>
+      <c r="C43">
+        <v>2.0531538724763321</v>
+      </c>
+      <c r="D43">
+        <v>5642.65</v>
+      </c>
+      <c r="E43">
+        <v>1.7327079271007659</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B44">
+        <v>720000982</v>
+      </c>
+      <c r="C44">
+        <v>10.265769362381659</v>
+      </c>
+      <c r="D44">
+        <v>28121.87</v>
+      </c>
+      <c r="E44">
+        <v>1.7215092935118965</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B45">
+        <v>720000982</v>
+      </c>
+      <c r="C45">
+        <v>25.66442340595415</v>
+      </c>
+      <c r="D45">
+        <v>69937.69</v>
+      </c>
+      <c r="E45">
+        <v>1.7174521146796908</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B46">
+        <v>720000982</v>
+      </c>
+      <c r="C46">
+        <v>49.7547621763431</v>
+      </c>
+      <c r="D46">
+        <v>138057.72</v>
+      </c>
+      <c r="E46">
+        <v>1.7077330934600388</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B47">
+        <v>720000982</v>
+      </c>
+      <c r="C47">
+        <v>74.632143264514653</v>
+      </c>
+      <c r="D47">
+        <v>210043.12</v>
+      </c>
+      <c r="E47">
+        <v>1.7374322581883261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B48">
+        <v>720000982</v>
+      </c>
+      <c r="C48">
+        <v>149.26428652902931</v>
+      </c>
+      <c r="D48">
+        <v>421187.11000000004</v>
+      </c>
+      <c r="E48">
+        <v>1.7211319297805721</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B49">
+        <v>720000982</v>
+      </c>
+      <c r="C49">
+        <v>298.52857305805861</v>
+      </c>
+      <c r="D49">
+        <v>855083.89</v>
+      </c>
+      <c r="E49">
+        <v>1.7147182650373909</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>